<commit_message>
save progress (next: OutputPotentialData.jl)
</commit_message>
<xml_diff>
--- a/Fitting Parameters/parameters.xlsx
+++ b/Fitting Parameters/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinno\OneDrive\progmrams\Guleria2012\Fitting Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ed250f2050058a0/progmrams/Guleria2012/Fitting Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B1A4A-A784-47FF-B843-092769D612BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{693B1A4A-A784-47FF-B843-092769D612BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B122261-5323-4901-AA11-B0183527FB3A}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>a1</t>
     <phoneticPr fontId="1"/>
@@ -211,13 +211,35 @@
   </si>
   <si>
     <t>GKW3_medium(rho&lt;1.5)</t>
+  </si>
+  <si>
+    <t>2022/10/21 momentum dependence refit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GKW2_lower(rho&lt;1.5)+Kohno2(k&lt;1.5)</t>
+  </si>
+  <si>
+    <t>GKW2_upper(rho&lt;1.5)+Kohno2(k&lt;1.5)</t>
+  </si>
+  <si>
+    <t>GKW2_medium(rho&lt;1.5)+Kohno2(k&lt;1.5)</t>
+  </si>
+  <si>
+    <t>GKW3_lower(rho&lt;1.5)+Kohno3(k&lt;1.5)</t>
+  </si>
+  <si>
+    <t>GKW3_upper(rho&lt;1.5)+Kohno3(k&lt;1.5)</t>
+  </si>
+  <si>
+    <t>GKW3_medium(rho&lt;1.5)+Kohno3(k&lt;1.5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +276,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -291,6 +319,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -571,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1302,7 +1331,7 @@
         <v>-352.20837441816951</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:K18" si="30">(C16+C17)/2</f>
+        <f t="shared" ref="C18:J18" si="30">(C16+C17)/2</f>
         <v>0</v>
       </c>
       <c r="D18">
@@ -1715,6 +1744,291 @@
       <c r="K28" s="6">
         <f t="shared" ref="K28" si="43">(K26+K27)*0.5</f>
         <v>3290.9645679995865</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="7">
+        <v>-397.00010084534301</v>
+      </c>
+      <c r="C31" s="5">
+        <v>39.350482632122898</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>-188.150449117742</v>
+      </c>
+      <c r="F31" s="5">
+        <v>835.75971860847199</v>
+      </c>
+      <c r="G31" s="2">
+        <f>B31</f>
+        <v>-397.00010084534301</v>
+      </c>
+      <c r="H31" s="2">
+        <f>C31</f>
+        <v>39.350482632122898</v>
+      </c>
+      <c r="I31" s="2">
+        <f>3*H31</f>
+        <v>118.0514478963687</v>
+      </c>
+      <c r="J31" s="2">
+        <f>8/3*F31</f>
+        <v>2228.692582955925</v>
+      </c>
+      <c r="K31" s="2">
+        <f>8/3*F31</f>
+        <v>2228.692582955925</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="7">
+        <v>-307.416648045557</v>
+      </c>
+      <c r="C32" s="5">
+        <v>39.350482632122898</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>-525.74679876459902</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1165.8672804160999</v>
+      </c>
+      <c r="G32" s="2">
+        <f>B32</f>
+        <v>-307.416648045557</v>
+      </c>
+      <c r="H32" s="2">
+        <f>C32</f>
+        <v>39.350482632122898</v>
+      </c>
+      <c r="I32" s="2">
+        <f>3*H32</f>
+        <v>118.0514478963687</v>
+      </c>
+      <c r="J32" s="2">
+        <f>8/3*F32</f>
+        <v>3108.9794144429329</v>
+      </c>
+      <c r="K32" s="2">
+        <f>8/3*F32</f>
+        <v>3108.9794144429329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="6">
+        <f>(B31+B32)/2</f>
+        <v>-352.20837444544998</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" ref="C33:K33" si="44">(C31+C32)/2</f>
+        <v>39.350482632122898</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="44"/>
+        <v>-356.94862394117052</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" si="44"/>
+        <v>1000.8134995122859</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="44"/>
+        <v>-352.20837444544998</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="44"/>
+        <v>39.350482632122898</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="44"/>
+        <v>118.0514478963687</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="44"/>
+        <v>2668.8359986994292</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="44"/>
+        <v>2668.8359986994292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="7">
+        <v>-414.44314258998099</v>
+      </c>
+      <c r="C34" s="5">
+        <v>47.278660369469797</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>-296.37382725478898</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1141.0537487988499</v>
+      </c>
+      <c r="G34" s="2">
+        <f>B34</f>
+        <v>-414.44314258998099</v>
+      </c>
+      <c r="H34" s="2">
+        <f>C34</f>
+        <v>47.278660369469797</v>
+      </c>
+      <c r="I34" s="2">
+        <f>3*H34</f>
+        <v>141.83598110840938</v>
+      </c>
+      <c r="J34" s="2">
+        <f>8/3*F34</f>
+        <v>3042.8099967969329</v>
+      </c>
+      <c r="K34" s="2">
+        <f>8/3*F34</f>
+        <v>3042.8099967969329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="7">
+        <v>-362.11045496717401</v>
+      </c>
+      <c r="C35" s="5">
+        <v>47.278660369469797</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>-514.970841835893</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1372.4455948611501</v>
+      </c>
+      <c r="G35" s="2">
+        <f>B35</f>
+        <v>-362.11045496717401</v>
+      </c>
+      <c r="H35" s="2">
+        <f>C35</f>
+        <v>47.278660369469797</v>
+      </c>
+      <c r="I35" s="2">
+        <f>3*H35</f>
+        <v>141.83598110840938</v>
+      </c>
+      <c r="J35" s="2">
+        <f>8/3*F35</f>
+        <v>3659.8549196297336</v>
+      </c>
+      <c r="K35" s="2">
+        <f>8/3*F35</f>
+        <v>3659.8549196297336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="6">
+        <f>(B34+B35)/2</f>
+        <v>-388.27679877857747</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" ref="C36" si="45">(C34+C35)/2</f>
+        <v>47.278660369469797</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" ref="D36" si="46">(D34+D35)/2</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" ref="E36" si="47">(E34+E35)/2</f>
+        <v>-405.67233454534096</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" ref="F36" si="48">(F34+F35)/2</f>
+        <v>1256.7496718299999</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" ref="G36" si="49">(G34+G35)/2</f>
+        <v>-388.27679877857747</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" ref="H36" si="50">(H34+H35)/2</f>
+        <v>47.278660369469797</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" ref="I36" si="51">(I34+I35)/2</f>
+        <v>141.83598110840938</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" ref="J36" si="52">(J34+J35)/2</f>
+        <v>3351.3324582133332</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" ref="K36" si="53">(K34+K35)/2</f>
+        <v>3351.3324582133332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>